<commit_message>
945 Grading criteria complete
</commit_message>
<xml_diff>
--- a/inst/adlb_grading_spec.xlsx
+++ b/inst/adlb_grading_spec.xlsx
@@ -700,9 +700,6 @@
     <t>TERM</t>
   </si>
   <si>
-    <t>IMPLEMENTATION</t>
-  </si>
-  <si>
     <t>SI_UNIT_CHECK</t>
   </si>
   <si>
@@ -1099,6 +1096,9 @@
 (!is.na(ANRHI) &amp; AVAL &lt;= ANRHI &amp; !is.na(BASE) &amp; AVAL &lt;= BASE) ~ "0",
 is.na(ANRHI) | is.na(BASE) ~ NA_character_
 )</t>
+  </si>
+  <si>
+    <t>GRADE_CRITERIA_CODE</t>
   </si>
 </sst>
 </file>
@@ -1459,8 +1459,8 @@
   </sheetPr>
   <dimension ref="A1:Z975"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" topLeftCell="F30" workbookViewId="0">
+      <selection activeCell="K30" sqref="K30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1500,19 +1500,19 @@
         <v>6</v>
       </c>
       <c r="I1" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="J1" s="4" t="s">
         <v>207</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>208</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>209</v>
       </c>
       <c r="L1" s="4" t="s">
         <v>187</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="N1" s="5"/>
       <c r="O1" s="5"/>
@@ -1606,7 +1606,7 @@
         <v>12</v>
       </c>
       <c r="I3" s="8" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="J3" s="11" t="s">
         <v>11</v>
@@ -1858,7 +1858,7 @@
         <v>38</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="J8" s="12"/>
       <c r="K8" s="4" t="s">
@@ -1960,7 +1960,7 @@
         <v>50</v>
       </c>
       <c r="I10" s="8" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="J10" s="14" t="s">
         <v>46</v>
@@ -2062,7 +2062,7 @@
         <v>62</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="J12" s="12"/>
       <c r="K12" s="4" t="s">
@@ -2112,7 +2112,7 @@
         <v>67</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="J13" s="4" t="s">
         <v>2</v>
@@ -2264,7 +2264,7 @@
         <v>202</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J16" s="4" t="s">
         <v>2</v>
@@ -2316,7 +2316,7 @@
         <v>82</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="J17" s="12"/>
       <c r="K17" s="4" t="s">
@@ -2326,7 +2326,7 @@
         <v>13</v>
       </c>
       <c r="M17" s="3" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="N17" s="5"/>
       <c r="O17" s="5"/>
@@ -2418,7 +2418,7 @@
         <v>91</v>
       </c>
       <c r="I19" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="J19" s="11" t="s">
         <v>11</v>
@@ -2470,7 +2470,7 @@
         <v>205</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="J20" s="11" t="s">
         <v>11</v>
@@ -2522,7 +2522,7 @@
         <v>100</v>
       </c>
       <c r="I21" s="8" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="J21" s="11" t="s">
         <v>11</v>
@@ -2574,7 +2574,7 @@
         <v>106</v>
       </c>
       <c r="I22" s="8" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="J22" s="11" t="s">
         <v>11</v>
@@ -2676,7 +2676,7 @@
         <v>114</v>
       </c>
       <c r="I24" s="8" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="J24" s="11" t="s">
         <v>11</v>
@@ -2704,7 +2704,7 @@
     </row>
     <row r="25" spans="1:26" ht="113" x14ac:dyDescent="0.3">
       <c r="A25" s="15" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B25" s="15" t="s">
         <v>115</v>
@@ -2725,13 +2725,13 @@
         <v>191</v>
       </c>
       <c r="H25" s="18" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J25" s="17" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="K25" s="4" t="s">
         <v>16</v>
@@ -2740,7 +2740,7 @@
         <v>13</v>
       </c>
       <c r="M25" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="N25" s="5"/>
       <c r="O25" s="5"/>
@@ -2758,10 +2758,10 @@
     </row>
     <row r="26" spans="1:26" ht="113" x14ac:dyDescent="0.3">
       <c r="A26" s="15" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B26" s="15" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C26" s="19" t="s">
         <v>116</v>
@@ -2779,13 +2779,13 @@
         <v>191</v>
       </c>
       <c r="H26" s="18" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="J26" s="17" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="K26" s="4" t="s">
         <v>16</v>
@@ -2794,7 +2794,7 @@
         <v>13</v>
       </c>
       <c r="M26" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="N26" s="5"/>
       <c r="O26" s="5"/>
@@ -2812,10 +2812,10 @@
     </row>
     <row r="27" spans="1:26" ht="113" x14ac:dyDescent="0.3">
       <c r="A27" s="16" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B27" s="16" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C27" s="20" t="s">
         <v>121</v>
@@ -2833,13 +2833,13 @@
         <v>191</v>
       </c>
       <c r="H27" s="18" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="J27" s="17" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="K27" s="4" t="s">
         <v>16</v>
@@ -2848,7 +2848,7 @@
         <v>13</v>
       </c>
       <c r="M27" s="3" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="N27" s="5"/>
       <c r="O27" s="5"/>
@@ -2866,7 +2866,7 @@
     </row>
     <row r="28" spans="1:26" ht="75.5" x14ac:dyDescent="0.3">
       <c r="A28" s="16" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B28" s="16" t="s">
         <v>120</v>
@@ -2887,13 +2887,13 @@
         <v>191</v>
       </c>
       <c r="H28" s="18" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="J28" s="17" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="K28" s="4" t="s">
         <v>4</v>
@@ -2902,7 +2902,7 @@
         <v>13</v>
       </c>
       <c r="M28" s="3" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="N28" s="5"/>
       <c r="O28" s="5"/>
@@ -2920,7 +2920,7 @@
     </row>
     <row r="29" spans="1:26" ht="113" x14ac:dyDescent="0.3">
       <c r="A29" s="16" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B29" s="16" t="s">
         <v>125</v>
@@ -2941,13 +2941,13 @@
         <v>191</v>
       </c>
       <c r="H29" s="18" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="J29" s="17" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="K29" s="4" t="s">
         <v>16</v>
@@ -2972,7 +2972,7 @@
     </row>
     <row r="30" spans="1:26" ht="100.5" x14ac:dyDescent="0.3">
       <c r="A30" s="16" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B30" s="16" t="s">
         <v>130</v>
@@ -2981,7 +2981,7 @@
         <v>131</v>
       </c>
       <c r="D30" s="20" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E30" s="20" t="s">
         <v>132</v>
@@ -2993,13 +2993,13 @@
         <v>191</v>
       </c>
       <c r="H30" s="18" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="J30" s="17" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="K30" s="4" t="s">
         <v>16</v>
@@ -3024,7 +3024,7 @@
     </row>
     <row r="31" spans="1:26" ht="113" x14ac:dyDescent="0.3">
       <c r="A31" s="16" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B31" s="16" t="s">
         <v>134</v>
@@ -3045,13 +3045,13 @@
         <v>191</v>
       </c>
       <c r="H31" s="18" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="J31" s="17" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="K31" s="4" t="s">
         <v>16</v>
@@ -3076,7 +3076,7 @@
     </row>
     <row r="32" spans="1:26" ht="100.5" x14ac:dyDescent="0.3">
       <c r="A32" s="16" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B32" s="16" t="s">
         <v>139</v>
@@ -3097,13 +3097,13 @@
         <v>191</v>
       </c>
       <c r="H32" s="18" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="J32" s="17" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="K32" s="4" t="s">
         <v>4</v>
@@ -3128,7 +3128,7 @@
     </row>
     <row r="33" spans="1:26" ht="88" x14ac:dyDescent="0.3">
       <c r="A33" s="15" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B33" s="15" t="s">
         <v>144</v>
@@ -3137,7 +3137,7 @@
         <v>145</v>
       </c>
       <c r="D33" s="19" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E33" s="19" t="s">
         <v>146</v>
@@ -3149,13 +3149,13 @@
         <v>191</v>
       </c>
       <c r="H33" s="18" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="J33" s="17" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="K33" s="4" t="s">
         <v>16</v>
@@ -3164,7 +3164,7 @@
         <v>13</v>
       </c>
       <c r="M33" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N33" s="5"/>
       <c r="O33" s="5"/>
@@ -3182,7 +3182,7 @@
     </row>
     <row r="34" spans="1:26" ht="100.5" x14ac:dyDescent="0.3">
       <c r="A34" s="16" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B34" s="16" t="s">
         <v>148</v>
@@ -3203,10 +3203,10 @@
         <v>191</v>
       </c>
       <c r="H34" s="18" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="J34" s="17" t="s">
         <v>2</v>
@@ -3234,7 +3234,7 @@
     </row>
     <row r="35" spans="1:26" ht="113" x14ac:dyDescent="0.3">
       <c r="A35" s="15" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B35" s="15" t="s">
         <v>152</v>
@@ -3255,13 +3255,13 @@
         <v>191</v>
       </c>
       <c r="H35" s="18" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="J35" s="17" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="K35" s="4" t="s">
         <v>3</v>
@@ -3270,7 +3270,7 @@
         <v>8</v>
       </c>
       <c r="M35" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="N35" s="5"/>
       <c r="O35" s="5"/>
@@ -3288,10 +3288,10 @@
     </row>
     <row r="36" spans="1:26" ht="113" x14ac:dyDescent="0.3">
       <c r="A36" s="15" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B36" s="15" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C36" s="19" t="s">
         <v>153</v>
@@ -3309,13 +3309,13 @@
         <v>191</v>
       </c>
       <c r="H36" s="18" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="J36" s="17" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="K36" s="4" t="s">
         <v>3</v>
@@ -3324,7 +3324,7 @@
         <v>8</v>
       </c>
       <c r="M36" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="N36" s="5"/>
       <c r="O36" s="5"/>
@@ -3342,7 +3342,7 @@
     </row>
     <row r="37" spans="1:26" ht="113" x14ac:dyDescent="0.3">
       <c r="A37" s="16" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B37" s="16" t="s">
         <v>157</v>
@@ -3363,13 +3363,13 @@
         <v>191</v>
       </c>
       <c r="H37" s="18" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="J37" s="17" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="K37" s="4" t="s">
         <v>3</v>
@@ -3394,7 +3394,7 @@
     </row>
     <row r="38" spans="1:26" ht="100.5" x14ac:dyDescent="0.3">
       <c r="A38" s="16" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B38" s="16" t="s">
         <v>162</v>
@@ -3415,13 +3415,13 @@
         <v>191</v>
       </c>
       <c r="H38" s="18" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="J38" s="17" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="K38" s="4" t="s">
         <v>3</v>
@@ -3430,7 +3430,7 @@
         <v>8</v>
       </c>
       <c r="M38" s="3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="N38" s="5"/>
       <c r="O38" s="5"/>
@@ -3448,7 +3448,7 @@
     </row>
     <row r="39" spans="1:26" ht="113" x14ac:dyDescent="0.3">
       <c r="A39" s="16" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B39" s="16" t="s">
         <v>167</v>
@@ -3469,13 +3469,13 @@
         <v>191</v>
       </c>
       <c r="H39" s="18" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="J39" s="17" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="K39" s="4" t="s">
         <v>3</v>
@@ -3500,7 +3500,7 @@
     </row>
     <row r="40" spans="1:26" ht="100.5" x14ac:dyDescent="0.3">
       <c r="A40" s="16" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B40" s="16" t="s">
         <v>172</v>
@@ -3509,7 +3509,7 @@
         <v>173</v>
       </c>
       <c r="D40" s="20" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E40" s="20" t="s">
         <v>174</v>
@@ -3521,13 +3521,13 @@
         <v>191</v>
       </c>
       <c r="H40" s="18" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J40" s="17" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="K40" s="4" t="s">
         <v>3</v>
@@ -3552,7 +3552,7 @@
     </row>
     <row r="41" spans="1:26" ht="113" x14ac:dyDescent="0.3">
       <c r="A41" s="16" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B41" s="16" t="s">
         <v>176</v>
@@ -3573,13 +3573,13 @@
         <v>191</v>
       </c>
       <c r="H41" s="18" t="s">
+        <v>234</v>
+      </c>
+      <c r="I41" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="J41" s="17" t="s">
         <v>235</v>
-      </c>
-      <c r="I41" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="J41" s="17" t="s">
-        <v>236</v>
       </c>
       <c r="K41" s="4" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
1202 ADLB scipt finalised for grading
</commit_message>
<xml_diff>
--- a/inst/adlb_grading_spec.xlsx
+++ b/inst/adlb_grading_spec.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\admiral\inst\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\admiral\inst\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1459,8 +1459,8 @@
   </sheetPr>
   <dimension ref="A1:Z975"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F30" workbookViewId="0">
-      <selection activeCell="K30" sqref="K30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1615,7 +1615,7 @@
         <v>4</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="M3" s="3"/>
       <c r="N3" s="5"/>

</xml_diff>